<commit_message>
base code for using DEAP
</commit_message>
<xml_diff>
--- a/xlsx_files/CM Freshmen.xlsx
+++ b/xlsx_files/CM Freshmen.xlsx
@@ -43,7 +43,7 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -58,8 +58,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D0CECE"/>
-        <bgColor rgb="00D0CECE"/>
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -72,12 +72,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -132,18 +126,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -578,21 +569,21 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>English Writing for Media
-09:00-10:30
-room:Creative room: 104</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
           <t>Russian Language (Elementary Level)
 09:00-10:30
 room:Creative room: 104</t>
         </is>
       </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Russian Language (Intermediate Level)
+09:00-10:30
+room:Creative room: 104</t>
+        </is>
+      </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>Russian Language (Beginner Level)
+          <t>Sociology
 09:00-10:30
 room:Creative room: 104</t>
         </is>
@@ -694,13 +685,6 @@
 room:Creative room: 104</t>
         </is>
       </c>
-      <c r="D14" s="5" t="inlineStr">
-        <is>
-          <t>Sociology
-11:00-12:30
-room:Creative room: 104</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
@@ -710,7 +694,6 @@
       </c>
       <c r="B15" s="6" t="n"/>
       <c r="C15" s="6" t="n"/>
-      <c r="D15" s="6" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -720,7 +703,6 @@
       </c>
       <c r="B16" s="6" t="n"/>
       <c r="C16" s="6" t="n"/>
-      <c r="D16" s="6" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
@@ -730,7 +712,6 @@
       </c>
       <c r="B17" s="6" t="n"/>
       <c r="C17" s="6" t="n"/>
-      <c r="D17" s="6" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -740,7 +721,6 @@
       </c>
       <c r="B18" s="6" t="n"/>
       <c r="C18" s="6" t="n"/>
-      <c r="D18" s="6" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -750,7 +730,6 @@
       </c>
       <c r="B19" s="7" t="n"/>
       <c r="C19" s="7" t="n"/>
-      <c r="D19" s="7" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -800,32 +779,25 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B26" s="8" t="inlineStr">
+      <c r="D26" s="5" t="inlineStr">
         <is>
           <t>Mathematics II
 14:00-15:30
-room:Grey classroom: 203</t>
-        </is>
-      </c>
-      <c r="D26" s="9" t="inlineStr">
-        <is>
-          <t>Russian Language (Elementary Level)
+room:White classroom: 202</t>
+        </is>
+      </c>
+      <c r="E26" s="8" t="inlineStr">
+        <is>
+          <t>English Writing for Media
 14:00-15:30
-room:Green classroom: 204</t>
-        </is>
-      </c>
-      <c r="E26" s="9" t="inlineStr">
-        <is>
-          <t>Media Literacy
+room:Yellow classroom: 209</t>
+        </is>
+      </c>
+      <c r="F26" s="8" t="inlineStr">
+        <is>
+          <t>English Writing for Media
 14:00-15:30
-room:Green classroom: 204</t>
-        </is>
-      </c>
-      <c r="F26" s="9" t="inlineStr">
-        <is>
-          <t>Mathematics II
-14:00-15:30
-room:Green classroom: 204</t>
+room:Yellow classroom: 209</t>
         </is>
       </c>
     </row>
@@ -835,7 +807,6 @@
           <t>14:15</t>
         </is>
       </c>
-      <c r="B27" s="6" t="n"/>
       <c r="D27" s="6" t="n"/>
       <c r="E27" s="6" t="n"/>
       <c r="F27" s="6" t="n"/>
@@ -846,7 +817,6 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B28" s="6" t="n"/>
       <c r="D28" s="6" t="n"/>
       <c r="E28" s="6" t="n"/>
       <c r="F28" s="6" t="n"/>
@@ -857,7 +827,6 @@
           <t>14:45</t>
         </is>
       </c>
-      <c r="B29" s="6" t="n"/>
       <c r="D29" s="6" t="n"/>
       <c r="E29" s="6" t="n"/>
       <c r="F29" s="6" t="n"/>
@@ -868,7 +837,6 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B30" s="6" t="n"/>
       <c r="D30" s="6" t="n"/>
       <c r="E30" s="6" t="n"/>
       <c r="F30" s="6" t="n"/>
@@ -879,7 +847,6 @@
           <t>15:15</t>
         </is>
       </c>
-      <c r="B31" s="7" t="n"/>
       <c r="D31" s="7" t="n"/>
       <c r="E31" s="7" t="n"/>
       <c r="F31" s="7" t="n"/>
@@ -904,27 +871,34 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="C34" s="9" t="inlineStr">
-        <is>
-          <t>English Writing for Media
-16:00-17:30
-room:Green classroom: 204</t>
-        </is>
-      </c>
-      <c r="E34" s="10" t="inlineStr">
+      <c r="B34" s="8" t="inlineStr">
         <is>
           <t>Russian Language (Beginner Level)
 16:00-17:30
 room:Yellow classroom: 209</t>
         </is>
       </c>
-      <c r="F34" s="10" t="inlineStr">
-        <is>
-          <t>Russian Language (Intermediate Level)
+      <c r="C34" s="8" t="inlineStr">
+        <is>
+          <t>Russian Language (Beginner Level)
 16:00-17:30
 room:Yellow classroom: 209</t>
         </is>
       </c>
+      <c r="E34" s="9" t="inlineStr">
+        <is>
+          <t>Media Literacy
+16:00-17:30
+room:Green classroom: 204</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>Russian Language (Elementary Level)
+16:00-17:30
+room:Yellow classroom: 209</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
@@ -932,6 +906,7 @@
           <t>16:15</t>
         </is>
       </c>
+      <c r="B35" s="6" t="n"/>
       <c r="C35" s="6" t="n"/>
       <c r="E35" s="6" t="n"/>
       <c r="F35" s="6" t="n"/>
@@ -942,6 +917,7 @@
           <t>16:30</t>
         </is>
       </c>
+      <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
       <c r="E36" s="6" t="n"/>
       <c r="F36" s="6" t="n"/>
@@ -952,6 +928,7 @@
           <t>16:45</t>
         </is>
       </c>
+      <c r="B37" s="6" t="n"/>
       <c r="C37" s="6" t="n"/>
       <c r="E37" s="6" t="n"/>
       <c r="F37" s="6" t="n"/>
@@ -962,6 +939,7 @@
           <t>17:00</t>
         </is>
       </c>
+      <c r="B38" s="6" t="n"/>
       <c r="C38" s="6" t="n"/>
       <c r="E38" s="6" t="n"/>
       <c r="F38" s="6" t="n"/>
@@ -972,6 +950,7 @@
           <t>17:15</t>
         </is>
       </c>
+      <c r="B39" s="7" t="n"/>
       <c r="C39" s="7" t="n"/>
       <c r="E39" s="7" t="n"/>
       <c r="F39" s="7" t="n"/>
@@ -1166,10 +1145,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B26:B31"/>
+  <mergeCells count="20">
+    <mergeCell ref="D26:D31"/>
     <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D26:D31"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="F3:F4"/>
@@ -1184,10 +1162,10 @@
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="F26:F31"/>
     <mergeCell ref="E6:E11"/>
+    <mergeCell ref="B34:B39"/>
     <mergeCell ref="E26:E31"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D14:D19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned version of GA
</commit_message>
<xml_diff>
--- a/xlsx_files/CM Freshmen.xlsx
+++ b/xlsx_files/CM Freshmen.xlsx
@@ -58,14 +58,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D0CECE"/>
-        <bgColor rgb="00D0CECE"/>
+        <fgColor rgb="0092D050"/>
+        <bgColor rgb="0092D050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0092D050"/>
-        <bgColor rgb="0092D050"/>
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -76,14 +76,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="00D0CECE"/>
+        <bgColor rgb="00D0CECE"/>
       </patternFill>
     </fill>
   </fills>
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -141,15 +141,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -582,18 +585,25 @@
           <t>09:00</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Mathematics II
+09:00-10:30
+room:204</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>Sociology
 09:00-10:30
 room:203</t>
         </is>
       </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>Media Literacy
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>Mathematics II
 09:00-10:30
-room:204</t>
+room:202</t>
         </is>
       </c>
     </row>
@@ -603,8 +613,9 @@
           <t>09:15</t>
         </is>
       </c>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="8" t="n"/>
+      <c r="E7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -612,8 +623,9 @@
           <t>09:30</t>
         </is>
       </c>
-      <c r="E8" s="7" t="n"/>
-      <c r="F8" s="7" t="n"/>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="8" t="n"/>
+      <c r="E8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -621,8 +633,9 @@
           <t>09:45</t>
         </is>
       </c>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
+      <c r="B9" s="8" t="n"/>
+      <c r="C9" s="8" t="n"/>
+      <c r="E9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -630,8 +643,9 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
+      <c r="B10" s="8" t="n"/>
+      <c r="C10" s="8" t="n"/>
+      <c r="E10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -639,8 +653,9 @@
           <t>10:15</t>
         </is>
       </c>
-      <c r="E11" s="8" t="n"/>
-      <c r="F11" s="8" t="n"/>
+      <c r="B11" s="9" t="n"/>
+      <c r="C11" s="9" t="n"/>
+      <c r="E11" s="9" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -662,32 +677,11 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>Mathematics II
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Russian Language (Intermediate Level)
 11:00-12:30
-room:203</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>Sociology
-11:00-12:30
-room:203</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="inlineStr">
-        <is>
-          <t>Physical training
-11:00-13:00
-room:100</t>
-        </is>
-      </c>
-      <c r="F14" s="9" t="inlineStr">
-        <is>
-          <t>Media Literacy
-11:00-12:30
-room:202</t>
+room:204</t>
         </is>
       </c>
     </row>
@@ -697,10 +691,7 @@
           <t>11:15</t>
         </is>
       </c>
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="7" t="n"/>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="7" t="n"/>
+      <c r="C15" s="8" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -708,10 +699,7 @@
           <t>11:30</t>
         </is>
       </c>
-      <c r="B16" s="7" t="n"/>
-      <c r="C16" s="7" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="7" t="n"/>
+      <c r="C16" s="8" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
@@ -719,10 +707,7 @@
           <t>11:45</t>
         </is>
       </c>
-      <c r="B17" s="7" t="n"/>
-      <c r="C17" s="7" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
+      <c r="C17" s="8" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -730,10 +715,7 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B18" s="7" t="n"/>
-      <c r="C18" s="7" t="n"/>
-      <c r="E18" s="7" t="n"/>
-      <c r="F18" s="7" t="n"/>
+      <c r="C18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -741,10 +723,7 @@
           <t>12:15</t>
         </is>
       </c>
-      <c r="B19" s="8" t="n"/>
-      <c r="C19" s="8" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="C19" s="9" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -752,7 +731,6 @@
           <t>12:30</t>
         </is>
       </c>
-      <c r="E20" s="7" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
@@ -760,7 +738,6 @@
           <t>12:45</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -796,18 +773,11 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>Russian Language (Beginner Level)
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>Media Literacy
 14:00-15:30
-room:201</t>
-        </is>
-      </c>
-      <c r="E26" s="6" t="inlineStr">
-        <is>
-          <t>Russian Language (Intermediate Level)
-14:00-15:30
-room:204</t>
+room:202</t>
         </is>
       </c>
     </row>
@@ -817,8 +787,7 @@
           <t>14:15</t>
         </is>
       </c>
-      <c r="B27" s="7" t="n"/>
-      <c r="E27" s="7" t="n"/>
+      <c r="D27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
@@ -826,8 +795,7 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B28" s="7" t="n"/>
-      <c r="E28" s="7" t="n"/>
+      <c r="D28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
@@ -835,8 +803,7 @@
           <t>14:45</t>
         </is>
       </c>
-      <c r="B29" s="7" t="n"/>
-      <c r="E29" s="7" t="n"/>
+      <c r="D29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
@@ -844,8 +811,7 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B30" s="7" t="n"/>
-      <c r="E30" s="7" t="n"/>
+      <c r="D30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
@@ -853,8 +819,7 @@
           <t>15:15</t>
         </is>
       </c>
-      <c r="B31" s="8" t="n"/>
-      <c r="E31" s="8" t="n"/>
+      <c r="D31" s="9" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
@@ -876,20 +841,41 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B34" s="6" t="inlineStr">
-        <is>
-          <t>Russian Language (Intermediate Level)
-16:00-17:30
-room:204</t>
-        </is>
-      </c>
-      <c r="E34" s="5" t="inlineStr">
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>Physical training
+16:00-18:00
+room:100</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
         <is>
           <t>Russian Language (Elementary Level)
 16:00-17:30
 room:203</t>
         </is>
       </c>
+      <c r="D34" s="10" t="inlineStr">
+        <is>
+          <t>Russian Language (Beginner Level)
+16:00-17:30
+room:209</t>
+        </is>
+      </c>
+      <c r="E34" s="10" t="inlineStr">
+        <is>
+          <t>Media Literacy
+16:00-17:30
+room:209</t>
+        </is>
+      </c>
+      <c r="F34" s="11" t="inlineStr">
+        <is>
+          <t>Sociology
+16:00-17:30
+room:201</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
@@ -897,8 +883,11 @@
           <t>16:15</t>
         </is>
       </c>
-      <c r="B35" s="7" t="n"/>
-      <c r="E35" s="7" t="n"/>
+      <c r="B35" s="8" t="n"/>
+      <c r="C35" s="8" t="n"/>
+      <c r="D35" s="8" t="n"/>
+      <c r="E35" s="8" t="n"/>
+      <c r="F35" s="8" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
@@ -906,8 +895,11 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="B36" s="7" t="n"/>
-      <c r="E36" s="7" t="n"/>
+      <c r="B36" s="8" t="n"/>
+      <c r="C36" s="8" t="n"/>
+      <c r="D36" s="8" t="n"/>
+      <c r="E36" s="8" t="n"/>
+      <c r="F36" s="8" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
@@ -915,8 +907,11 @@
           <t>16:45</t>
         </is>
       </c>
-      <c r="B37" s="7" t="n"/>
-      <c r="E37" s="7" t="n"/>
+      <c r="B37" s="8" t="n"/>
+      <c r="C37" s="8" t="n"/>
+      <c r="D37" s="8" t="n"/>
+      <c r="E37" s="8" t="n"/>
+      <c r="F37" s="8" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -924,8 +919,11 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B38" s="7" t="n"/>
-      <c r="E38" s="7" t="n"/>
+      <c r="B38" s="8" t="n"/>
+      <c r="C38" s="8" t="n"/>
+      <c r="D38" s="8" t="n"/>
+      <c r="E38" s="8" t="n"/>
+      <c r="F38" s="8" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -934,7 +932,10 @@
         </is>
       </c>
       <c r="B39" s="8" t="n"/>
-      <c r="E39" s="8" t="n"/>
+      <c r="C39" s="9" t="n"/>
+      <c r="D39" s="9" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
@@ -942,6 +943,7 @@
           <t>17:30</t>
         </is>
       </c>
+      <c r="B40" s="8" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
@@ -949,6 +951,7 @@
           <t>17:45</t>
         </is>
       </c>
+      <c r="B41" s="9" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
@@ -1126,24 +1129,25 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="E26:E31"/>
+  <mergeCells count="18">
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="B34:B41"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B6:B11"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="F34:F39"/>
     <mergeCell ref="B34:B39"/>
-    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="C14:C19"/>
     <mergeCell ref="E34:E39"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F6:F11"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="F14:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>